<commit_message>
Assembled case, new calibr data
</commit_message>
<xml_diff>
--- a/Look up table.xlsx
+++ b/Look up table.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucac\Desktop\Luca\PoliMi\Magistrale\II anno\Electronic technologies and biosensors laboratory\Projects\AY2122_II_Project-2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucac\Desktop\Luca\PoliMi\Magistrale\II anno\ETBL\Projects\AY2122_II_Project-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB435F4E-8F3F-4C14-ACBA-E2C34F9F5D19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A0D1B80-6C2B-43B0-8A64-614C3D614365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{D8641024-8F43-455E-9147-D99A6BDD0C2E}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>CHRONOAMPEROMETRY</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t>Picco CV [mV]</t>
+  </si>
+  <si>
+    <t>CASE</t>
   </si>
 </sst>
 </file>
@@ -105,7 +108,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -115,6 +118,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -132,7 +141,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -140,19 +149,41 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -470,43 +501,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A4D8310-A7A9-429A-8F7A-A57DF4043D90}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="28.88671875" customWidth="1"/>
-    <col min="2" max="2" width="19.33203125" customWidth="1"/>
-    <col min="3" max="3" width="17.88671875" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.88671875" style="1" customWidth="1"/>
     <col min="6" max="6" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="4"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F2" s="9"/>
+      <c r="I2" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>80</v>
       </c>
@@ -516,14 +550,14 @@
       <c r="C3" s="1">
         <v>2484</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="5">
         <v>1800</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="4">
         <v>2800</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>80</v>
       </c>
@@ -533,187 +567,392 @@
       <c r="C4" s="1">
         <v>2508</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <v>1800</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <v>2800</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>80</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="6">
         <v>1.65</v>
       </c>
       <c r="C5" s="1">
         <v>2414</v>
       </c>
-      <c r="D5">
-        <f>SUM(B3:B5)/3</f>
-        <v>1.8666666666666665</v>
-      </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>1800</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <v>2800</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
+        <v>80</v>
+      </c>
+      <c r="B6" s="8">
+        <v>2.1</v>
+      </c>
+      <c r="C6" s="1">
+        <v>402</v>
+      </c>
+      <c r="D6">
+        <f>SUM(B3:B6)/4</f>
+        <v>1.9249999999999998</v>
+      </c>
+      <c r="E6" s="5">
+        <v>-400</v>
+      </c>
+      <c r="F6" s="4">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="11">
+        <v>80</v>
+      </c>
+      <c r="B7" s="12">
+        <v>1.6</v>
+      </c>
+      <c r="C7" s="11">
+        <v>178</v>
+      </c>
+      <c r="D7" s="13"/>
+      <c r="E7" s="14">
+        <v>-400</v>
+      </c>
+      <c r="F7" s="15">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="11">
+        <v>80</v>
+      </c>
+      <c r="B8" s="12">
+        <v>1.75</v>
+      </c>
+      <c r="C8" s="11">
+        <v>102</v>
+      </c>
+      <c r="D8" s="13"/>
+      <c r="E8" s="14">
+        <v>-400</v>
+      </c>
+      <c r="F8" s="15">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>100</v>
+      </c>
+      <c r="B9" s="8">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="C9" s="1">
+        <v>452</v>
+      </c>
+      <c r="E9" s="5">
+        <v>-400</v>
+      </c>
+      <c r="F9" s="4">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>100</v>
+      </c>
+      <c r="B10" s="8"/>
+      <c r="E10" s="5">
+        <v>-400</v>
+      </c>
+      <c r="F10" s="4">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>100</v>
+      </c>
+      <c r="B11" s="8"/>
+      <c r="E11" s="5">
+        <v>-400</v>
+      </c>
+      <c r="F11" s="4">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>100</v>
+      </c>
+      <c r="B12" s="8"/>
+      <c r="E12" s="5">
+        <v>-400</v>
+      </c>
+      <c r="F12" s="4">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="11">
+        <v>100</v>
+      </c>
+      <c r="B13" s="12"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="15"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="11">
+        <v>100</v>
+      </c>
+      <c r="B14" s="12"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="15"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
         <v>115</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B15" s="6">
         <v>2.2999999999999998</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C15" s="1">
         <v>2434</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E15" s="5">
         <v>1800</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F15" s="4">
         <v>2800</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
         <v>115</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B16" s="6">
         <v>2.25</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C16" s="1">
         <v>2468</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E16" s="5">
         <v>1800</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F16" s="4">
         <v>2800</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
         <v>115</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B17" s="6">
         <v>2.2999999999999998</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C17" s="1">
         <v>2490</v>
       </c>
-      <c r="D8">
-        <f>SUM(B6:B8)/3</f>
-        <v>2.2833333333333332</v>
-      </c>
-      <c r="E8" s="6">
+      <c r="E17" s="5">
         <v>1800</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F17" s="4">
         <v>2800</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>115</v>
+      </c>
+      <c r="B18" s="8">
+        <v>3</v>
+      </c>
+      <c r="D18">
+        <f>SUM(B15:B18)/4</f>
+        <v>2.4624999999999999</v>
+      </c>
+      <c r="E18" s="5">
+        <v>-400</v>
+      </c>
+      <c r="F18" s="4">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>115</v>
+      </c>
+      <c r="B19" s="8">
+        <v>2.7</v>
+      </c>
+      <c r="C19" s="1">
+        <v>444</v>
+      </c>
+      <c r="E19" s="5">
+        <v>-400</v>
+      </c>
+      <c r="F19" s="4">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="11">
+        <v>115</v>
+      </c>
+      <c r="B20" s="12">
+        <v>1.95</v>
+      </c>
+      <c r="C20" s="11">
+        <v>178</v>
+      </c>
+      <c r="D20" s="13"/>
+      <c r="E20" s="5">
+        <v>-400</v>
+      </c>
+      <c r="F20" s="4">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="11">
+        <v>115</v>
+      </c>
+      <c r="B21" s="12">
+        <v>1.9</v>
+      </c>
+      <c r="C21" s="11">
+        <v>170</v>
+      </c>
+      <c r="D21" s="13"/>
+      <c r="E21" s="5">
+        <v>-400</v>
+      </c>
+      <c r="F21" s="4">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
         <v>150</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B22" s="6">
         <v>2.65</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C22" s="1">
         <v>2484</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E22" s="5">
         <v>1800</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F22" s="4">
         <v>2800</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
         <v>150</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B23" s="6">
         <v>2.5</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C23" s="1">
         <v>2476</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E23" s="5">
         <v>1800</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F23" s="4">
         <v>2800</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
         <v>150</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B24" s="6">
         <v>2.6</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C24" s="1">
         <v>2452</v>
       </c>
-      <c r="D11">
-        <f>SUM(B9:B11)/3</f>
-        <v>2.5833333333333335</v>
-      </c>
-      <c r="E11" s="6">
+      <c r="E24" s="5">
         <v>1800</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F24" s="4">
         <v>2800</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>150</v>
+      </c>
+      <c r="B25" s="8">
+        <v>4.3</v>
+      </c>
+      <c r="C25" s="1">
+        <v>470</v>
+      </c>
+      <c r="D25">
+        <f>SUM(B22:B25)/4</f>
+        <v>3.0125000000000002</v>
+      </c>
+      <c r="E25" s="5">
+        <v>-400</v>
+      </c>
+      <c r="F25" s="4">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="11">
+        <v>150</v>
+      </c>
+      <c r="B26" s="11">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C26" s="11">
+        <v>194</v>
+      </c>
+      <c r="D26" s="13"/>
+      <c r="E26" s="5">
+        <v>-400</v>
+      </c>
+      <c r="F26" s="4">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="11">
+        <v>150</v>
+      </c>
+      <c r="B27" s="11">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="C27" s="11">
+        <v>336</v>
+      </c>
+      <c r="D27" s="13"/>
+      <c r="E27" s="5">
+        <v>-400</v>
+      </c>
+      <c r="F27" s="4">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
New calibration and presentation
</commit_message>
<xml_diff>
--- a/Look up table.xlsx
+++ b/Look up table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucac\Desktop\Luca\PoliMi\Magistrale\II anno\ETBL\Projects\AY2122_II_Project-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A0D1B80-6C2B-43B0-8A64-614C3D614365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D25D75CF-FE36-4FA9-8EBC-A4F41563A93C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{D8641024-8F43-455E-9147-D99A6BDD0C2E}"/>
   </bookViews>
@@ -167,12 +167,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -184,6 +178,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -501,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A4D8310-A7A9-429A-8F7A-A57DF4043D90}">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -516,11 +516,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -532,11 +532,11 @@
       <c r="C2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="9"/>
-      <c r="I2" s="11" t="s">
+      <c r="F2" s="14"/>
+      <c r="I2" s="9" t="s">
         <v>5</v>
       </c>
     </row>
@@ -613,38 +613,38 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="11">
+      <c r="A7" s="9">
         <v>80</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="10">
         <v>1.6</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="9">
         <v>178</v>
       </c>
-      <c r="D7" s="13"/>
-      <c r="E7" s="14">
-        <v>-400</v>
-      </c>
-      <c r="F7" s="15">
+      <c r="D7" s="11"/>
+      <c r="E7" s="12">
+        <v>-400</v>
+      </c>
+      <c r="F7" s="13">
         <v>800</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="11">
+      <c r="A8" s="9">
         <v>80</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8" s="10">
         <v>1.75</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="9">
         <v>102</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="14">
-        <v>-400</v>
-      </c>
-      <c r="F8" s="15">
+      <c r="D8" s="11"/>
+      <c r="E8" s="12">
+        <v>-400</v>
+      </c>
+      <c r="F8" s="13">
         <v>800</v>
       </c>
     </row>
@@ -702,24 +702,24 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="11">
+      <c r="A13" s="9">
         <v>100</v>
       </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="15"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="13"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="11">
+      <c r="A14" s="9">
         <v>100</v>
       </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="15"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="13"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
@@ -808,16 +808,16 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="11">
+      <c r="A20" s="9">
         <v>115</v>
       </c>
-      <c r="B20" s="12">
+      <c r="B20" s="10">
         <v>1.95</v>
       </c>
-      <c r="C20" s="11">
+      <c r="C20" s="9">
         <v>178</v>
       </c>
-      <c r="D20" s="13"/>
+      <c r="D20" s="11"/>
       <c r="E20" s="5">
         <v>-400</v>
       </c>
@@ -826,16 +826,16 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="11">
+      <c r="A21" s="9">
         <v>115</v>
       </c>
-      <c r="B21" s="12">
+      <c r="B21" s="10">
         <v>1.9</v>
       </c>
-      <c r="C21" s="11">
+      <c r="C21" s="9">
         <v>170</v>
       </c>
-      <c r="D21" s="13"/>
+      <c r="D21" s="11"/>
       <c r="E21" s="5">
         <v>-400</v>
       </c>
@@ -844,20 +844,21 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="1">
-        <v>150</v>
-      </c>
-      <c r="B22" s="6">
-        <v>2.65</v>
-      </c>
-      <c r="C22" s="1">
-        <v>2484</v>
-      </c>
+      <c r="A22" s="9">
+        <v>130</v>
+      </c>
+      <c r="B22" s="10">
+        <v>2.4</v>
+      </c>
+      <c r="C22" s="9">
+        <v>242</v>
+      </c>
+      <c r="D22" s="11"/>
       <c r="E22" s="5">
-        <v>1800</v>
+        <v>-400</v>
       </c>
       <c r="F22" s="4">
-        <v>2800</v>
+        <v>800</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -865,10 +866,10 @@
         <v>150</v>
       </c>
       <c r="B23" s="6">
-        <v>2.5</v>
+        <v>2.65</v>
       </c>
       <c r="C23" s="1">
-        <v>2476</v>
+        <v>2484</v>
       </c>
       <c r="E23" s="5">
         <v>1800</v>
@@ -882,10 +883,10 @@
         <v>150</v>
       </c>
       <c r="B24" s="6">
-        <v>2.6</v>
+        <v>2.5</v>
       </c>
       <c r="C24" s="1">
-        <v>2452</v>
+        <v>2476</v>
       </c>
       <c r="E24" s="5">
         <v>1800</v>
@@ -898,61 +899,78 @@
       <c r="A25" s="1">
         <v>150</v>
       </c>
-      <c r="B25" s="8">
+      <c r="B25" s="6">
+        <v>2.6</v>
+      </c>
+      <c r="C25" s="1">
+        <v>2452</v>
+      </c>
+      <c r="E25" s="5">
+        <v>1800</v>
+      </c>
+      <c r="F25" s="4">
+        <v>2800</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>150</v>
+      </c>
+      <c r="B26" s="8">
         <v>4.3</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C26" s="1">
         <v>470</v>
       </c>
-      <c r="D25">
-        <f>SUM(B22:B25)/4</f>
+      <c r="D26">
+        <f>SUM(B23:B26)/4</f>
         <v>3.0125000000000002</v>
       </c>
-      <c r="E25" s="5">
-        <v>-400</v>
-      </c>
-      <c r="F25" s="4">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="11">
+      <c r="E26" s="5">
+        <v>-400</v>
+      </c>
+      <c r="F26" s="4">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="9">
         <v>150</v>
       </c>
-      <c r="B26" s="11">
+      <c r="B27" s="9">
         <v>2.2000000000000002</v>
       </c>
-      <c r="C26" s="11">
+      <c r="C27" s="9">
         <v>194</v>
       </c>
-      <c r="D26" s="13"/>
-      <c r="E26" s="5">
-        <v>-400</v>
-      </c>
-      <c r="F26" s="4">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="11">
+      <c r="D27" s="11"/>
+      <c r="E27" s="5">
+        <v>-400</v>
+      </c>
+      <c r="F27" s="4">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="9">
         <v>150</v>
       </c>
-      <c r="B27" s="11">
+      <c r="B28" s="9">
         <v>2.4500000000000002</v>
       </c>
-      <c r="C27" s="11">
+      <c r="C28" s="9">
         <v>336</v>
       </c>
-      <c r="D27" s="13"/>
-      <c r="E27" s="5">
-        <v>-400</v>
-      </c>
-      <c r="F27" s="4">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="1"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="5">
+        <v>-400</v>
+      </c>
+      <c r="F28" s="4">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>